<commit_message>
fixed missing species name issues
</commit_message>
<xml_diff>
--- a/20231026-master_metadata_file-curated.xlsx
+++ b/20231026-master_metadata_file-curated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konrad/Desktop/Segre_lab/202206-Marine_strain_collection/iamm-collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B735F54-94A6-1040-8B53-2959DC00374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907243CF-F124-F841-B04E-40BFA0832AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="812">
   <si>
     <t>ds_strain_id</t>
   </si>
@@ -1099,9 +1099,6 @@
     <t>inhibens</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>Kolter lab</t>
   </si>
   <si>
@@ -2386,9 +2383,6 @@
     <t>D20-160070-4500T</t>
   </si>
   <si>
-    <t>Sulfitobacter pseudonitzschiae (Luca1)</t>
-  </si>
-  <si>
     <t>Nitsch</t>
   </si>
   <si>
@@ -2459,6 +2453,9 @@
   </si>
   <si>
     <t>nitzsch/smr1</t>
+  </si>
+  <si>
+    <t>Luca1</t>
   </si>
 </sst>
 </file>
@@ -2781,9 +2778,9 @@
   </sheetPr>
   <dimension ref="A1:Y983"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R76" sqref="R76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4196,7 +4193,7 @@
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>67</v>
@@ -4265,7 +4262,7 @@
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>67</v>
@@ -5336,21 +5333,21 @@
         <v>358</v>
       </c>
       <c r="R40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S40" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="T40" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="T40" s="4" t="s">
+      <c r="U40" s="4" t="s">
         <v>361</v>
-      </c>
-      <c r="U40" s="4" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>329</v>
@@ -5378,7 +5375,7 @@
         <v>50</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>28</v>
@@ -5387,33 +5384,33 @@
         <v>134</v>
       </c>
       <c r="N41" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="O41" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="O41" s="4" t="s">
+      <c r="P41" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="P41" s="4" t="s">
+      <c r="Q41" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="Q41" s="4" t="s">
+      <c r="R41" s="4" t="s">
         <v>368</v>
-      </c>
-      <c r="R41" s="4" t="s">
-        <v>369</v>
       </c>
       <c r="S41" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="U41" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>329</v>
@@ -5441,7 +5438,7 @@
         <v>50</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>28</v>
@@ -5456,13 +5453,13 @@
         <v>168</v>
       </c>
       <c r="P42" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q42" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="Q42" s="4" t="s">
+      <c r="R42" s="4" t="s">
         <v>374</v>
-      </c>
-      <c r="R42" s="4" t="s">
-        <v>375</v>
       </c>
       <c r="S42" s="4" t="s">
         <v>91</v>
@@ -5471,12 +5468,12 @@
         <v>50</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>329</v>
@@ -5504,7 +5501,7 @@
         <v>50</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>28</v>
@@ -5519,27 +5516,27 @@
         <v>168</v>
       </c>
       <c r="P43" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q43" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="Q43" s="4" t="s">
+      <c r="R43" s="4" t="s">
         <v>380</v>
-      </c>
-      <c r="R43" s="4" t="s">
-        <v>381</v>
       </c>
       <c r="S43" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T43" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="U43" s="4" t="s">
         <v>382</v>
-      </c>
-      <c r="U43" s="4" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>329</v>
@@ -5567,7 +5564,7 @@
         <v>50</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>251</v>
@@ -5582,27 +5579,27 @@
         <v>252</v>
       </c>
       <c r="P44" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q44" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="Q44" s="4" t="s">
+      <c r="R44" s="4" t="s">
         <v>387</v>
-      </c>
-      <c r="R44" s="4" t="s">
-        <v>388</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="U44" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>329</v>
@@ -5630,7 +5627,7 @@
         <v>50</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>51</v>
@@ -5642,30 +5639,30 @@
         <v>116</v>
       </c>
       <c r="O45" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="P45" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="Q45" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="Q45" s="4" t="s">
+      <c r="R45" s="4" t="s">
         <v>394</v>
-      </c>
-      <c r="R45" s="4" t="s">
-        <v>395</v>
       </c>
       <c r="S45" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="U45" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>329</v>
@@ -5693,7 +5690,7 @@
         <v>50</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>51</v>
@@ -5708,13 +5705,13 @@
         <v>117</v>
       </c>
       <c r="P46" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q46" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="Q46" s="4" t="s">
+      <c r="R46" s="4" t="s">
         <v>400</v>
-      </c>
-      <c r="R46" s="4" t="s">
-        <v>401</v>
       </c>
       <c r="S46" s="4" t="s">
         <v>234</v>
@@ -5723,12 +5720,12 @@
         <v>50</v>
       </c>
       <c r="U46" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>329</v>
@@ -5756,7 +5753,7 @@
         <v>50</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>51</v>
@@ -5771,27 +5768,27 @@
         <v>117</v>
       </c>
       <c r="P47" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q47" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="Q47" s="4" t="s">
+      <c r="R47" s="4" t="s">
         <v>406</v>
-      </c>
-      <c r="R47" s="4" t="s">
-        <v>407</v>
       </c>
       <c r="S47" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T47" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="U47" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>329</v>
@@ -5840,7 +5837,7 @@
         <v>101</v>
       </c>
       <c r="R48" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="S48" s="8" t="s">
         <v>91</v>
@@ -5849,7 +5846,7 @@
         <v>50</v>
       </c>
       <c r="U48" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
@@ -5858,7 +5855,7 @@
     </row>
     <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>329</v>
@@ -5907,21 +5904,21 @@
         <v>214</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="S49" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T49" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="U49" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>329</v>
@@ -5949,7 +5946,7 @@
         <v>50</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>28</v>
@@ -5964,10 +5961,10 @@
         <v>212</v>
       </c>
       <c r="P50" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q50" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="Q50" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="R50" s="4" t="s">
         <v>50</v>
@@ -5976,15 +5973,15 @@
         <v>35</v>
       </c>
       <c r="T50" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="U50" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>329</v>
@@ -6012,7 +6009,7 @@
         <v>50</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>28</v>
@@ -6021,33 +6018,33 @@
         <v>29</v>
       </c>
       <c r="N51" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="O51" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="O51" s="4" t="s">
+      <c r="P51" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="P51" s="4" t="s">
+      <c r="Q51" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="R51" s="4" t="s">
         <v>422</v>
-      </c>
-      <c r="Q51" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="R51" s="4" t="s">
-        <v>423</v>
       </c>
       <c r="S51" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T51" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="U51" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>329</v>
@@ -6075,7 +6072,7 @@
         <v>50</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L52" s="12" t="s">
         <v>28</v>
@@ -6087,25 +6084,25 @@
         <v>80</v>
       </c>
       <c r="O52" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="P52" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="P52" s="12" t="s">
+      <c r="Q52" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="R52" s="12" t="s">
         <v>428</v>
-      </c>
-      <c r="Q52" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="R52" s="12" t="s">
-        <v>429</v>
       </c>
       <c r="S52" s="12" t="s">
         <v>85</v>
       </c>
       <c r="T52" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="U52" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="U52" s="12" t="s">
-        <v>431</v>
       </c>
       <c r="V52" s="13"/>
       <c r="W52" s="13"/>
@@ -6114,7 +6111,7 @@
     </row>
     <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>329</v>
@@ -6142,7 +6139,7 @@
         <v>50</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>28</v>
@@ -6157,27 +6154,27 @@
         <v>29</v>
       </c>
       <c r="P53" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q53" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="Q53" s="4" t="s">
+      <c r="R53" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="R53" s="4" t="s">
-        <v>436</v>
       </c>
       <c r="S53" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T53" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="U53" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>329</v>
@@ -6205,7 +6202,7 @@
         <v>50</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>28</v>
@@ -6220,13 +6217,13 @@
         <v>168</v>
       </c>
       <c r="P54" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q54" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="Q54" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="R54" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="S54" s="4" t="s">
         <v>58</v>
@@ -6235,12 +6232,12 @@
         <v>50</v>
       </c>
       <c r="U54" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>329</v>
@@ -6268,7 +6265,7 @@
         <v>50</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>28</v>
@@ -6277,33 +6274,33 @@
         <v>29</v>
       </c>
       <c r="N55" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="O55" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="O55" s="4" t="s">
+      <c r="P55" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="P55" s="4" t="s">
+      <c r="Q55" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="Q55" s="4" t="s">
+      <c r="R55" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="R55" s="4" t="s">
-        <v>448</v>
       </c>
       <c r="S55" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T55" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="U55" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>329</v>
@@ -6331,7 +6328,7 @@
         <v>50</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>28</v>
@@ -6343,30 +6340,30 @@
         <v>80</v>
       </c>
       <c r="O56" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="P56" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="P56" s="4" t="s">
+      <c r="Q56" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="Q56" s="4" t="s">
+      <c r="R56" s="4" t="s">
         <v>454</v>
-      </c>
-      <c r="R56" s="4" t="s">
-        <v>455</v>
       </c>
       <c r="S56" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T56" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="U56" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>329</v>
@@ -6394,7 +6391,7 @@
         <v>50</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>28</v>
@@ -6406,30 +6403,30 @@
         <v>80</v>
       </c>
       <c r="O57" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="P57" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="P57" s="4" t="s">
-        <v>453</v>
-      </c>
       <c r="Q57" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="R57" s="4" t="s">
         <v>459</v>
-      </c>
-      <c r="R57" s="4" t="s">
-        <v>460</v>
       </c>
       <c r="S57" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T57" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="U57" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="U57" s="4" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>329</v>
@@ -6457,7 +6454,7 @@
         <v>50</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L58" s="4" t="s">
         <v>28</v>
@@ -6472,13 +6469,13 @@
         <v>168</v>
       </c>
       <c r="P58" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q58" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="Q58" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="R58" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="S58" s="4" t="s">
         <v>120</v>
@@ -6487,12 +6484,12 @@
         <v>50</v>
       </c>
       <c r="U58" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>329</v>
@@ -6520,7 +6517,7 @@
         <v>50</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L59" s="4" t="s">
         <v>28</v>
@@ -6532,30 +6529,30 @@
         <v>80</v>
       </c>
       <c r="O59" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="P59" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="P59" s="4" t="s">
-        <v>428</v>
-      </c>
       <c r="Q59" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="R59" s="4" t="s">
         <v>468</v>
-      </c>
-      <c r="R59" s="4" t="s">
-        <v>469</v>
       </c>
       <c r="S59" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T59" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="U59" s="4" t="s">
         <v>470</v>
-      </c>
-      <c r="U59" s="4" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>329</v>
@@ -6583,42 +6580,42 @@
         <v>50</v>
       </c>
       <c r="K60" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="L60" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="L60" s="4" t="s">
+      <c r="M60" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="M60" s="4" t="s">
+      <c r="N60" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="N60" s="4" t="s">
+      <c r="O60" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="O60" s="4" t="s">
+      <c r="P60" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="P60" s="4" t="s">
+      <c r="Q60" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="Q60" s="4" t="s">
+      <c r="R60" s="4" t="s">
         <v>479</v>
-      </c>
-      <c r="R60" s="4" t="s">
-        <v>480</v>
       </c>
       <c r="S60" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T60" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="U60" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="U60" s="4" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>329</v>
@@ -6646,7 +6643,7 @@
         <v>50</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L61" s="4" t="s">
         <v>28</v>
@@ -6658,30 +6655,30 @@
         <v>50</v>
       </c>
       <c r="O61" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="P61" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="P61" s="4" t="s">
+      <c r="Q61" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="Q61" s="4" t="s">
+      <c r="R61" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="R61" s="4" t="s">
+      <c r="S61" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="S61" s="4" t="s">
+      <c r="T61" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="T61" s="4" t="s">
-        <v>490</v>
-      </c>
       <c r="U61" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>329</v>
@@ -6709,42 +6706,42 @@
         <v>50</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L62" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M62" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="N62" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="N62" s="4" t="s">
+      <c r="O62" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="O62" s="4" t="s">
+      <c r="P62" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="P62" s="4" t="s">
+      <c r="Q62" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="R62" s="4" t="s">
         <v>496</v>
-      </c>
-      <c r="Q62" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="R62" s="4" t="s">
-        <v>497</v>
       </c>
       <c r="S62" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T62" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="U62" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="U62" s="4" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>329</v>
@@ -6772,7 +6769,7 @@
         <v>50</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L63" s="4" t="s">
         <v>28</v>
@@ -6781,16 +6778,16 @@
         <v>29</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O63" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="P63" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="P63" s="4" t="s">
-        <v>503</v>
-      </c>
       <c r="Q63" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="R63" s="4" t="s">
         <v>91</v>
@@ -6799,15 +6796,15 @@
         <v>35</v>
       </c>
       <c r="T63" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U63" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>329</v>
@@ -6835,42 +6832,42 @@
         <v>50</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L64" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M64" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="N64" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="N64" s="4" t="s">
+      <c r="O64" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="O64" s="4" t="s">
+      <c r="P64" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="P64" s="4" t="s">
+      <c r="Q64" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="Q64" s="4" t="s">
+      <c r="R64" s="4" t="s">
         <v>511</v>
-      </c>
-      <c r="R64" s="4" t="s">
-        <v>512</v>
       </c>
       <c r="S64" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T64" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="U64" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="65" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>329</v>
@@ -6898,7 +6895,7 @@
         <v>50</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L65" s="4" t="s">
         <v>28</v>
@@ -6916,10 +6913,10 @@
         <v>310</v>
       </c>
       <c r="Q65" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="R65" s="4" t="s">
         <v>516</v>
-      </c>
-      <c r="R65" s="4" t="s">
-        <v>517</v>
       </c>
       <c r="S65" s="4" t="s">
         <v>120</v>
@@ -6928,12 +6925,12 @@
         <v>50</v>
       </c>
       <c r="U65" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="66" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>329</v>
@@ -6961,7 +6958,7 @@
         <v>50</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L66" s="4" t="s">
         <v>28</v>
@@ -6970,33 +6967,33 @@
         <v>29</v>
       </c>
       <c r="N66" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="O66" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="O66" s="4" t="s">
+      <c r="P66" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="P66" s="4" t="s">
+      <c r="Q66" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="Q66" s="4" t="s">
+      <c r="R66" s="4" t="s">
         <v>524</v>
-      </c>
-      <c r="R66" s="4" t="s">
-        <v>525</v>
       </c>
       <c r="S66" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T66" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="U66" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>329</v>
@@ -7024,7 +7021,7 @@
         <v>50</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L67" s="4" t="s">
         <v>28</v>
@@ -7039,13 +7036,13 @@
         <v>168</v>
       </c>
       <c r="P67" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q67" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="Q67" s="4" t="s">
+      <c r="R67" s="4" t="s">
         <v>530</v>
-      </c>
-      <c r="R67" s="4" t="s">
-        <v>531</v>
       </c>
       <c r="S67" s="4" t="s">
         <v>120</v>
@@ -7054,12 +7051,12 @@
         <v>50</v>
       </c>
       <c r="U67" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="68" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>329</v>
@@ -7087,42 +7084,42 @@
         <v>50</v>
       </c>
       <c r="K68" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="L68" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="L68" s="4" t="s">
+      <c r="M68" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="N68" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="M68" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="N68" s="4" t="s">
+      <c r="O68" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="O68" s="4" t="s">
+      <c r="P68" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="P68" s="4" t="s">
+      <c r="Q68" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="Q68" s="4" t="s">
+      <c r="R68" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="R68" s="4" t="s">
-        <v>540</v>
       </c>
       <c r="S68" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T68" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="U68" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="69" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>329</v>
@@ -7150,7 +7147,7 @@
         <v>50</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L69" s="4" t="s">
         <v>28</v>
@@ -7159,33 +7156,33 @@
         <v>29</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O69" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="P69" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q69" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="Q69" s="4" t="s">
+      <c r="R69" s="4" t="s">
         <v>545</v>
-      </c>
-      <c r="R69" s="4" t="s">
-        <v>546</v>
       </c>
       <c r="S69" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T69" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="U69" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>22</v>
@@ -7194,25 +7191,25 @@
         <v>89</v>
       </c>
       <c r="E70" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I70" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="F70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I70" s="4" t="s">
+      <c r="J70" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K70" s="4" t="s">
         <v>550</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>551</v>
       </c>
       <c r="L70" s="4" t="s">
         <v>28</v>
@@ -7227,13 +7224,13 @@
         <v>168</v>
       </c>
       <c r="P70" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q70" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="Q70" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="R70" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="S70" s="4" t="s">
         <v>58</v>
@@ -7242,12 +7239,12 @@
         <v>50</v>
       </c>
       <c r="U70" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>22</v>
@@ -7256,25 +7253,25 @@
         <v>91</v>
       </c>
       <c r="E71" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I71" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="F71" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I71" s="4" t="s">
+      <c r="J71" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="J71" s="4" t="s">
+      <c r="K71" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="K71" s="4" t="s">
-        <v>556</v>
       </c>
       <c r="L71" s="4" t="s">
         <v>28</v>
@@ -7289,13 +7286,13 @@
         <v>168</v>
       </c>
       <c r="P71" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q71" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="Q71" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="R71" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="S71" s="4" t="s">
         <v>58</v>
@@ -7304,12 +7301,12 @@
         <v>50</v>
       </c>
       <c r="U71" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>22</v>
@@ -7318,25 +7315,25 @@
         <v>92</v>
       </c>
       <c r="E72" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I72" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I72" s="4" t="s">
+      <c r="J72" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="K72" s="4" t="s">
         <v>559</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="K72" s="4" t="s">
-        <v>560</v>
       </c>
       <c r="L72" s="4" t="s">
         <v>28</v>
@@ -7351,13 +7348,13 @@
         <v>168</v>
       </c>
       <c r="P72" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q72" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="Q72" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="R72" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="S72" s="4" t="s">
         <v>58</v>
@@ -7366,12 +7363,12 @@
         <v>50</v>
       </c>
       <c r="U72" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>22</v>
@@ -7380,25 +7377,25 @@
         <v>93</v>
       </c>
       <c r="E73" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I73" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="F73" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I73" s="4" t="s">
+      <c r="J73" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="K73" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="K73" s="4" t="s">
-        <v>564</v>
       </c>
       <c r="L73" s="4" t="s">
         <v>28</v>
@@ -7413,13 +7410,13 @@
         <v>168</v>
       </c>
       <c r="P73" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q73" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="Q73" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="R73" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="S73" s="4" t="s">
         <v>58</v>
@@ -7428,12 +7425,12 @@
         <v>50</v>
       </c>
       <c r="U73" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>22</v>
@@ -7443,25 +7440,25 @@
         <v>66</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="F74" s="4" t="s">
-        <v>567</v>
-      </c>
       <c r="G74" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L74" s="4" t="s">
         <v>28</v>
@@ -7476,57 +7473,57 @@
         <v>168</v>
       </c>
       <c r="P74" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q74" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="Q74" s="4" t="s">
+      <c r="R74" s="4" t="s">
         <v>570</v>
-      </c>
-      <c r="R74" s="4" t="s">
-        <v>571</v>
       </c>
       <c r="S74" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T74" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="U74" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D75" s="5">
         <v>51</v>
       </c>
       <c r="E75" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="G75" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="G75" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="I75" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="J75" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="I75" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>579</v>
-      </c>
       <c r="K75" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L75" s="4" t="s">
         <v>28</v>
@@ -7538,60 +7535,60 @@
         <v>135</v>
       </c>
       <c r="O75" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="P75" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="P75" s="4" t="s">
+      <c r="Q75" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="Q75" s="4" t="s">
+      <c r="R75" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="S75" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="R75" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="S75" s="4" t="s">
+      <c r="T75" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U75" s="4" t="s">
         <v>583</v>
-      </c>
-      <c r="T75" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U75" s="4" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D76" s="5">
         <v>52</v>
       </c>
       <c r="E76" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="F76" s="4" t="s">
+      <c r="G76" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="G76" s="4" t="s">
+      <c r="H76" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="H76" s="4" t="s">
+      <c r="I76" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="J76" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="I76" s="4" t="s">
-        <v>589</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>591</v>
-      </c>
       <c r="K76" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L76" s="4" t="s">
         <v>28</v>
@@ -7609,51 +7606,51 @@
         <v>357</v>
       </c>
       <c r="Q76" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="R76" s="4" t="s">
-        <v>359</v>
+        <v>50</v>
       </c>
       <c r="S76" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T76" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="U76" s="4" t="s">
         <v>593</v>
-      </c>
-      <c r="U76" s="4" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="77" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D77" s="5">
         <v>84</v>
       </c>
       <c r="E77" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="F77" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="F77" s="4" t="s">
+      <c r="G77" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="G77" s="4" t="s">
+      <c r="H77" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I77" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="H77" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I77" s="4" t="s">
+      <c r="J77" s="4" t="s">
         <v>600</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>601</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>50</v>
@@ -7683,7 +7680,7 @@
         <v>35</v>
       </c>
       <c r="T77" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="U77" s="4" t="s">
         <v>50</v>
@@ -7691,34 +7688,34 @@
     </row>
     <row r="78" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D78" s="5">
         <v>86</v>
       </c>
       <c r="E78" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="G78" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="H78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I78" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="H78" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I78" s="4" t="s">
+      <c r="J78" s="4" t="s">
         <v>607</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>608</v>
       </c>
       <c r="K78" s="4" t="s">
         <v>50</v>
@@ -7748,7 +7745,7 @@
         <v>35</v>
       </c>
       <c r="T78" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="U78" s="4" t="s">
         <v>50</v>
@@ -7756,7 +7753,7 @@
     </row>
     <row r="79" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>22</v>
@@ -7766,25 +7763,25 @@
         <v>53</v>
       </c>
       <c r="E79" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="F79" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="F79" s="4" t="s">
+      <c r="G79" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>613</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I79" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="J79" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="J79" s="4" t="s">
-        <v>614</v>
-      </c>
       <c r="K79" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="L79" s="4" t="s">
         <v>28</v>
@@ -7799,27 +7796,27 @@
         <v>81</v>
       </c>
       <c r="P79" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q79" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="Q79" s="4" t="s">
+      <c r="R79" s="4" t="s">
         <v>616</v>
-      </c>
-      <c r="R79" s="4" t="s">
-        <v>617</v>
       </c>
       <c r="S79" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T79" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="U79" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>22</v>
@@ -7829,25 +7826,25 @@
         <v>39</v>
       </c>
       <c r="E80" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="F80" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="F80" s="4" t="s">
+      <c r="G80" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>622</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>50</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L80" s="4" t="s">
         <v>28</v>
@@ -7859,16 +7856,16 @@
         <v>80</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P80" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Q80" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="R80" s="4" t="s">
-        <v>359</v>
+        <v>50</v>
       </c>
       <c r="S80" s="4" t="s">
         <v>234</v>
@@ -7877,12 +7874,12 @@
         <v>50</v>
       </c>
       <c r="U80" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="81" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>22</v>
@@ -7892,25 +7889,25 @@
         <v>54</v>
       </c>
       <c r="E81" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F81" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="G81" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>627</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="J81" s="4" t="s">
-        <v>628</v>
-      </c>
       <c r="K81" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L81" s="4" t="s">
         <v>28</v>
@@ -7922,30 +7919,30 @@
         <v>135</v>
       </c>
       <c r="O81" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="P81" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="P81" s="4" t="s">
+      <c r="Q81" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="Q81" s="4" t="s">
-        <v>582</v>
-      </c>
       <c r="R81" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="S81" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T81" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="U81" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>22</v>
@@ -7955,25 +7952,25 @@
         <v>49</v>
       </c>
       <c r="E82" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="F82" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="G82" s="4" t="s">
         <v>632</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>633</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L82" s="4" t="s">
         <v>28</v>
@@ -7985,30 +7982,30 @@
         <v>80</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P82" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Q82" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="R82" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="R82" s="4" t="s">
+      <c r="S82" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="S82" s="4" t="s">
+      <c r="T82" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="T82" s="4" t="s">
-        <v>637</v>
-      </c>
       <c r="U82" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="83" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>22</v>
@@ -8018,60 +8015,60 @@
         <v>67</v>
       </c>
       <c r="E83" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="F83" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="G83" s="4" t="s">
         <v>640</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>641</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I83" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="J83" s="4" t="s">
         <v>641</v>
       </c>
-      <c r="J83" s="4" t="s">
-        <v>642</v>
-      </c>
       <c r="K83" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="L83" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M83" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="N83" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="N83" s="4" t="s">
+      <c r="O83" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="O83" s="4" t="s">
+      <c r="P83" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="P83" s="4" t="s">
+      <c r="Q83" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="Q83" s="4" t="s">
+      <c r="R83" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="R83" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="S83" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T83" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="U83" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="84" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>22</v>
@@ -8081,25 +8078,25 @@
         <v>60</v>
       </c>
       <c r="E84" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="F84" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="F84" s="4" t="s">
+      <c r="G84" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="G84" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I84" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="J84" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="J84" s="4" t="s">
-        <v>654</v>
-      </c>
       <c r="K84" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="L84" s="4" t="s">
         <v>28</v>
@@ -8108,60 +8105,60 @@
         <v>29</v>
       </c>
       <c r="N84" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="O84" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="O84" s="4" t="s">
+      <c r="P84" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="P84" s="4" t="s">
+      <c r="Q84" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="Q84" s="4" t="s">
+      <c r="R84" s="4" t="s">
         <v>658</v>
-      </c>
-      <c r="R84" s="4" t="s">
-        <v>659</v>
       </c>
       <c r="S84" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T84" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="U84" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="85" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D85" s="5">
         <v>75</v>
       </c>
       <c r="E85" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="G85" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="G85" s="4" t="s">
+      <c r="H85" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I85" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="H85" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I85" s="4" t="s">
+      <c r="J85" s="4" t="s">
         <v>666</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>667</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>50</v>
@@ -8191,7 +8188,7 @@
         <v>35</v>
       </c>
       <c r="T85" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="U85" s="4" t="s">
         <v>50</v>
@@ -8199,37 +8196,37 @@
     </row>
     <row r="86" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D86" s="5">
         <v>40</v>
       </c>
       <c r="E86" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="F86" s="4" t="s">
+      <c r="G86" s="4" t="s">
         <v>671</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>672</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I86" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="J86" s="4" t="s">
-        <v>673</v>
-      </c>
       <c r="K86" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L86" s="4" t="s">
         <v>28</v>
@@ -8244,27 +8241,27 @@
         <v>168</v>
       </c>
       <c r="P86" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q86" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="R86" s="4" t="s">
         <v>674</v>
-      </c>
-      <c r="R86" s="4" t="s">
-        <v>675</v>
       </c>
       <c r="S86" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T86" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="U86" s="4" t="s">
         <v>676</v>
-      </c>
-      <c r="U86" s="4" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="87" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>22</v>
@@ -8274,25 +8271,25 @@
         <v>64</v>
       </c>
       <c r="E87" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="F87" s="4" t="s">
-        <v>680</v>
-      </c>
       <c r="G87" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="L87" s="4" t="s">
         <v>146</v>
@@ -8304,57 +8301,57 @@
         <v>147</v>
       </c>
       <c r="O87" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="P87" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="P87" s="4" t="s">
+      <c r="Q87" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="Q87" s="4" t="s">
-        <v>684</v>
-      </c>
       <c r="R87" s="4" t="s">
-        <v>359</v>
+        <v>50</v>
       </c>
       <c r="S87" s="4" t="s">
         <v>294</v>
       </c>
       <c r="T87" s="4" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="U87" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="88" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="4" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D88" s="5">
         <v>77</v>
       </c>
       <c r="E88" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="F88" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="G88" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="G88" s="4" t="s">
+      <c r="H88" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I88" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="H88" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I88" s="4" t="s">
+      <c r="J88" s="4" t="s">
         <v>691</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>692</v>
       </c>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
@@ -8368,13 +8365,13 @@
         <v>35</v>
       </c>
       <c r="T88" s="4" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="U88" s="4"/>
     </row>
     <row r="89" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>22</v>
@@ -8384,25 +8381,25 @@
         <v>41</v>
       </c>
       <c r="E89" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="F89" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="G89" s="4" t="s">
         <v>695</v>
-      </c>
-      <c r="G89" s="4" t="s">
-        <v>696</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I89" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K89" s="4" t="s">
         <v>696</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K89" s="4" t="s">
-        <v>697</v>
       </c>
       <c r="L89" s="4" t="s">
         <v>28</v>
@@ -8417,13 +8414,13 @@
         <v>168</v>
       </c>
       <c r="P89" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q89" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="Q89" s="4" t="s">
+      <c r="R89" s="4" t="s">
         <v>699</v>
-      </c>
-      <c r="R89" s="4" t="s">
-        <v>700</v>
       </c>
       <c r="S89" s="4" t="s">
         <v>120</v>
@@ -8432,12 +8429,12 @@
         <v>50</v>
       </c>
       <c r="U89" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="90" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>22</v>
@@ -8447,25 +8444,25 @@
         <v>42</v>
       </c>
       <c r="E90" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="F90" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="F90" s="4" t="s">
+      <c r="G90" s="4" t="s">
         <v>703</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>704</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I90" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="J90" s="4" t="s">
-        <v>705</v>
-      </c>
       <c r="K90" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="L90" s="4" t="s">
         <v>28</v>
@@ -8480,54 +8477,54 @@
         <v>168</v>
       </c>
       <c r="P90" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q90" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="Q90" s="4" t="s">
+      <c r="R90" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="S90" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="R90" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="S90" s="4" t="s">
-        <v>708</v>
-      </c>
       <c r="T90" s="4" t="s">
         <v>50</v>
       </c>
       <c r="U90" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="91" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D91" s="5">
         <v>81</v>
       </c>
       <c r="E91" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="F91" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="F91" s="4" t="s">
+      <c r="G91" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="G91" s="4" t="s">
+      <c r="H91" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I91" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="H91" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I91" s="4" t="s">
+      <c r="J91" s="4" t="s">
         <v>714</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>715</v>
       </c>
       <c r="K91" s="4" t="s">
         <v>50</v>
@@ -8557,7 +8554,7 @@
         <v>35</v>
       </c>
       <c r="T91" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="U91" s="4" t="s">
         <v>50</v>
@@ -8565,34 +8562,34 @@
     </row>
     <row r="92" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D92" s="5">
         <v>72</v>
       </c>
       <c r="E92" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="F92" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="F92" s="4" t="s">
+      <c r="G92" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="G92" s="4" t="s">
+      <c r="H92" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I92" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="H92" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I92" s="4" t="s">
+      <c r="J92" s="4" t="s">
         <v>722</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>723</v>
       </c>
       <c r="K92" s="4" t="s">
         <v>50</v>
@@ -8622,7 +8619,7 @@
         <v>35</v>
       </c>
       <c r="T92" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="U92" s="4" t="s">
         <v>50</v>
@@ -8630,7 +8627,7 @@
     </row>
     <row r="93" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>22</v>
@@ -8639,25 +8636,25 @@
         <v>62</v>
       </c>
       <c r="E93" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="F93" s="4" t="s">
         <v>726</v>
       </c>
-      <c r="F93" s="4" t="s">
+      <c r="G93" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="G93" s="4" t="s">
+      <c r="H93" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="H93" s="4" t="s">
+      <c r="I93" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="I93" s="4" t="s">
-        <v>728</v>
-      </c>
-      <c r="J93" s="4" t="s">
-        <v>730</v>
-      </c>
       <c r="K93" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="L93" s="4" t="s">
         <v>28</v>
@@ -8669,54 +8666,54 @@
         <v>211</v>
       </c>
       <c r="O93" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="P93" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="P93" s="4" t="s">
+      <c r="Q93" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="R93" s="4" t="s">
         <v>732</v>
-      </c>
-      <c r="Q93" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="R93" s="4" t="s">
-        <v>733</v>
       </c>
       <c r="S93" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T93" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="U93" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="94" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="12" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D94" s="13">
         <v>55</v>
       </c>
       <c r="E94" s="13" t="s">
+        <v>735</v>
+      </c>
+      <c r="F94" s="12" t="s">
         <v>736</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="G94" s="12" t="s">
         <v>737</v>
       </c>
-      <c r="G94" s="12" t="s">
+      <c r="H94" s="12" t="s">
         <v>738</v>
       </c>
-      <c r="H94" s="12" t="s">
-        <v>739</v>
-      </c>
       <c r="I94" s="12" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J94" s="12" t="s">
         <v>50</v>
@@ -8741,7 +8738,7 @@
     </row>
     <row r="95" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>22</v>
@@ -8751,25 +8748,25 @@
         <v>43</v>
       </c>
       <c r="E95" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="F95" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="F95" s="4" t="s">
+      <c r="G95" s="4" t="s">
         <v>742</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>743</v>
       </c>
       <c r="H95" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I95" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="J95" s="4" t="s">
-        <v>744</v>
-      </c>
       <c r="K95" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="L95" s="4" t="s">
         <v>28</v>
@@ -8781,30 +8778,30 @@
         <v>80</v>
       </c>
       <c r="O95" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="P95" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="P95" s="4" t="s">
-        <v>428</v>
-      </c>
       <c r="Q95" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="R95" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="S95" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T95" s="4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="U95" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="96" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>22</v>
@@ -8814,25 +8811,25 @@
         <v>69</v>
       </c>
       <c r="E96" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="F96" s="4" t="s">
         <v>748</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="G96" s="4" t="s">
         <v>749</v>
-      </c>
-      <c r="G96" s="4" t="s">
-        <v>750</v>
       </c>
       <c r="H96" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I96" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="K96" s="4" t="s">
         <v>751</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>752</v>
       </c>
       <c r="L96" s="4" t="s">
         <v>28</v>
@@ -8841,63 +8838,63 @@
         <v>29</v>
       </c>
       <c r="N96" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="O96" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="P96" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="O96" s="4" t="s">
-        <v>753</v>
-      </c>
-      <c r="P96" s="4" t="s">
+      <c r="Q96" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="Q96" s="4" t="s">
+      <c r="R96" s="4" t="s">
         <v>755</v>
-      </c>
-      <c r="R96" s="4" t="s">
-        <v>756</v>
       </c>
       <c r="S96" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T96" s="4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="U96" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="97" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D97" s="5">
         <v>82</v>
       </c>
       <c r="E97" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="F97" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="F97" s="4" t="s">
+      <c r="G97" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="G97" s="4" t="s">
+      <c r="H97" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="J97" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K97" s="4" t="s">
         <v>762</v>
-      </c>
-      <c r="H97" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I97" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K97" s="4" t="s">
-        <v>763</v>
       </c>
       <c r="L97" s="4" t="s">
         <v>28</v>
@@ -8909,60 +8906,60 @@
         <v>135</v>
       </c>
       <c r="O97" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="P97" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="P97" s="4" t="s">
+      <c r="Q97" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="Q97" s="4" t="s">
+      <c r="R97" s="4" t="s">
         <v>766</v>
-      </c>
-      <c r="R97" s="4" t="s">
-        <v>767</v>
       </c>
       <c r="S97" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T97" s="4" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="U97" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="98" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D98" s="5">
         <v>44</v>
       </c>
       <c r="E98" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="F98" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="F98" s="4" t="s">
+      <c r="G98" s="4" t="s">
         <v>771</v>
       </c>
-      <c r="G98" s="4" t="s">
+      <c r="H98" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="H98" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I98" s="4" t="s">
-        <v>772</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>773</v>
-      </c>
       <c r="K98" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L98" s="4" t="s">
         <v>28</v>
@@ -8971,19 +8968,19 @@
         <v>134</v>
       </c>
       <c r="N98" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="O98" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="O98" s="4" t="s">
+      <c r="P98" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="P98" s="4" t="s">
+      <c r="Q98" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="Q98" s="4" t="s">
-        <v>777</v>
-      </c>
       <c r="R98" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="S98" s="4" t="s">
         <v>120</v>
@@ -8992,42 +8989,42 @@
         <v>50</v>
       </c>
       <c r="U98" s="4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="99" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D99" s="15">
         <v>45</v>
       </c>
       <c r="E99" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="F99" s="14" t="s">
         <v>781</v>
       </c>
-      <c r="F99" s="14" t="s">
+      <c r="G99" s="14" t="s">
         <v>782</v>
       </c>
-      <c r="G99" s="14" t="s">
-        <v>783</v>
-      </c>
       <c r="H99" s="14" t="s">
         <v>50</v>
       </c>
       <c r="I99" s="14" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J99" s="14" t="s">
         <v>50</v>
       </c>
       <c r="K99" s="14" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="L99" s="14" t="s">
         <v>28</v>
@@ -9042,13 +9039,13 @@
         <v>168</v>
       </c>
       <c r="P99" s="14" t="s">
+        <v>783</v>
+      </c>
+      <c r="Q99" s="14" t="s">
         <v>784</v>
       </c>
-      <c r="Q99" s="14" t="s">
-        <v>785</v>
-      </c>
       <c r="R99" s="14" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="S99" s="14" t="s">
         <v>120</v>
@@ -9057,7 +9054,7 @@
         <v>50</v>
       </c>
       <c r="U99" s="14" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="V99" s="15"/>
       <c r="W99" s="15"/>
@@ -9066,34 +9063,34 @@
     </row>
     <row r="100" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="14" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D100" s="15">
         <v>70</v>
       </c>
       <c r="E100" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>781</v>
+      </c>
+      <c r="G100" s="14" t="s">
+        <v>811</v>
+      </c>
+      <c r="H100" s="14" t="s">
+        <v>788</v>
+      </c>
+      <c r="I100" s="14" t="s">
         <v>787</v>
       </c>
-      <c r="F100" s="14" t="s">
-        <v>788</v>
-      </c>
-      <c r="G100" s="14" t="s">
+      <c r="J100" s="14" t="s">
         <v>789</v>
-      </c>
-      <c r="H100" s="14" t="s">
-        <v>790</v>
-      </c>
-      <c r="I100" s="14" t="s">
-        <v>789</v>
-      </c>
-      <c r="J100" s="14" t="s">
-        <v>791</v>
       </c>
       <c r="K100" s="14"/>
       <c r="L100" s="14"/>
@@ -9115,7 +9112,7 @@
     </row>
     <row r="101" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="4" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>22</v>
@@ -9125,25 +9122,25 @@
         <v>59</v>
       </c>
       <c r="E101" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>793</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>794</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>795</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I101" s="4" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="L101" s="4" t="s">
         <v>28</v>
@@ -9152,33 +9149,33 @@
         <v>29</v>
       </c>
       <c r="N101" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="O101" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="O101" s="4" t="s">
+      <c r="P101" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="P101" s="4" t="s">
-        <v>446</v>
-      </c>
       <c r="Q101" s="4" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="R101" s="4" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="S101" s="4" t="s">
         <v>35</v>
       </c>
       <c r="T101" s="4" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="U101" s="4" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="102" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>22</v>
@@ -9188,25 +9185,25 @@
         <v>46</v>
       </c>
       <c r="E102" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="G102" s="4" t="s">
         <v>801</v>
-      </c>
-      <c r="F102" s="4" t="s">
-        <v>802</v>
-      </c>
-      <c r="G102" s="4" t="s">
-        <v>803</v>
       </c>
       <c r="H102" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="K102" s="4" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="L102" s="4" t="s">
         <v>28</v>
@@ -9215,28 +9212,28 @@
         <v>29</v>
       </c>
       <c r="N102" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="O102" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="O102" s="4" t="s">
+      <c r="P102" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="P102" s="4" t="s">
-        <v>446</v>
-      </c>
       <c r="Q102" s="4" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="R102" s="4" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="S102" s="4" t="s">
         <v>85</v>
       </c>
       <c r="T102" s="4" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="U102" s="4" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="103" spans="1:25" ht="13" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fixed several strain matches
</commit_message>
<xml_diff>
--- a/20231026-master_metadata_file-curated.xlsx
+++ b/20231026-master_metadata_file-curated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konrad/Desktop/Segre_lab/202206-Marine_strain_collection/iamm-collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907243CF-F124-F841-B04E-40BFA0832AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE98E466-A0ED-1941-8AE5-7EB195E426B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="811">
   <si>
     <t>ds_strain_id</t>
   </si>
@@ -2450,9 +2450,6 @@
   </si>
   <si>
     <t>nitzsch/luca1</t>
-  </si>
-  <si>
-    <t>nitzsch/smr1</t>
   </si>
   <si>
     <t>Luca1</t>
@@ -2778,9 +2775,9 @@
   </sheetPr>
   <dimension ref="A1:Y983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R76" sqref="R76"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8994,7 +8991,7 @@
     </row>
     <row r="99" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="14" t="s">
-        <v>810</v>
+        <v>778</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>22</v>
@@ -9081,7 +9078,7 @@
         <v>781</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="H100" s="14" t="s">
         <v>788</v>

</xml_diff>